<commit_message>
Enhance README.md with detailed features, installation, usage instructions, and update package generation script to validate input file and open output directory automatically
</commit_message>
<xml_diff>
--- a/Metadatos.xlsx
+++ b/Metadatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosas\Mis cosas Web\salesforce-package-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E19F25-D8FA-4B91-B60C-C41215FE0BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB1CFC8-EF69-43E4-9A50-5572C59E7B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Tipo</t>
   </si>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,56 +567,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor generatePackage.js to improve metadata handling and enhance API mapping logic
</commit_message>
<xml_diff>
--- a/Metadatos.xlsx
+++ b/Metadatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosas\Mis cosas Web\salesforce-package-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB1CFC8-EF69-43E4-9A50-5572C59E7B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDD1EF-ED43-4073-A0F1-65B0F9761331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="735" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Meta</t>
-  </si>
-  <si>
-    <t>Api</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>lwc_test</t>
+  </si>
+  <si>
+    <t>MetadataType</t>
+  </si>
+  <si>
+    <t>ApiName</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,13 +442,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -458,113 +458,113 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor generatePackage.js to adjust API naming conventions and update package.xml to include new Layout type
</commit_message>
<xml_diff>
--- a/Metadatos.xlsx
+++ b/Metadatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cosas\Mis cosas Web\salesforce-package-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDD1EF-ED43-4073-A0F1-65B0F9761331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA72324-1B1F-4B02-B098-7BBC1D4F5CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4305" yWindow="735" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Tipo</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>ApiName</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Página Objeto</t>
+  </si>
+  <si>
+    <t>Objeto__c</t>
   </si>
 </sst>
 </file>
@@ -424,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +576,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>